<commit_message>
1-Check the Registration And Get the Exist Already Message
</commit_message>
<xml_diff>
--- a/src/test/java/Apache/Resource/schoolDepartment.xlsx
+++ b/src/test/java/Apache/Resource/schoolDepartment.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">karaLise</t>
+    <t xml:space="preserve">kara46lise</t>
   </si>
   <si>
-    <t xml:space="preserve">km46</t>
+    <t xml:space="preserve">kasu</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>